<commit_message>
Issue was solved by changing lcd24bpp to lcd32bpp
</commit_message>
<xml_diff>
--- a/User/TouchGFX/assets/texts/texts.xlsx
+++ b/User/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="71">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1652,24 +1652,24 @@
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
         <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
         <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
         <v>38</v>
@@ -1681,29 +1681,29 @@
         <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
         <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
@@ -1715,12 +1715,12 @@
         <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
@@ -1732,12 +1732,12 @@
         <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
@@ -1749,29 +1749,29 @@
         <v>45</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
         <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
@@ -1788,24 +1788,24 @@
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E12" t="s">
         <v>45</v>
       </c>
       <c r="F12" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
@@ -1817,12 +1817,12 @@
         <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
testing png file displaying
</commit_message>
<xml_diff>
--- a/User/TouchGFX/assets/texts/texts.xlsx
+++ b/User/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="71">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1669,7 +1669,7 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
         <v>38</v>
@@ -1681,46 +1681,46 @@
         <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
         <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
         <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
@@ -1732,29 +1732,29 @@
         <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
         <v>45</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
@@ -1766,29 +1766,29 @@
         <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
         <v>45</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
@@ -1800,41 +1800,41 @@
         <v>45</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
         <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
         <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>